<commit_message>
commit de formatação dos campos
</commit_message>
<xml_diff>
--- a/Empreendedorismo/Empreendedorismo - CANVAS.xlsx
+++ b/Empreendedorismo/Empreendedorismo - CANVAS.xlsx
@@ -171,12 +171,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,11 +213,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -236,22 +258,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -274,7 +291,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -289,38 +328,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -334,14 +356,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -349,11 +363,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -378,12 +392,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -396,7 +404,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,25 +488,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,13 +536,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,61 +560,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -522,43 +572,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -806,51 +820,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -871,11 +844,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -895,6 +874,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -903,155 +908,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="29" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1061,36 +1075,36 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1107,28 +1121,30 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -1149,6 +1165,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="58" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1174,9 +1204,8 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment vertical="center"/>
@@ -4002,8 +4031,8 @@
   </sheetPr>
   <dimension ref="B1:FD37"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="BR3" sqref="BR3:CR3"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="AI8" sqref="AI8:BK8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.28666666666667" defaultRowHeight="33" customHeight="1"/>
@@ -4309,17 +4338,17 @@
       <c r="CU3" s="37"/>
       <c r="CV3" s="37"/>
       <c r="CW3" s="37"/>
-      <c r="CX3" s="38">
+      <c r="CX3" s="42">
         <v>43226</v>
       </c>
-      <c r="CY3" s="39"/>
-      <c r="CZ3" s="39"/>
-      <c r="DA3" s="39"/>
-      <c r="DB3" s="39"/>
-      <c r="DC3" s="39"/>
-      <c r="DD3" s="39"/>
-      <c r="DE3" s="39"/>
-      <c r="DF3" s="40"/>
+      <c r="CY3" s="43"/>
+      <c r="CZ3" s="43"/>
+      <c r="DA3" s="43"/>
+      <c r="DB3" s="43"/>
+      <c r="DC3" s="43"/>
+      <c r="DD3" s="43"/>
+      <c r="DE3" s="43"/>
+      <c r="DF3" s="44"/>
       <c r="DG3" s="18"/>
       <c r="DH3" s="18"/>
       <c r="DI3" s="18"/>
@@ -4332,17 +4361,17 @@
       <c r="DN3" s="37"/>
       <c r="DO3" s="37"/>
       <c r="DP3" s="18"/>
-      <c r="DQ3" s="41" t="s">
+      <c r="DQ3" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="DR3" s="42"/>
-      <c r="DS3" s="42"/>
-      <c r="DT3" s="42"/>
-      <c r="DU3" s="42"/>
-      <c r="DV3" s="42"/>
-      <c r="DW3" s="42"/>
-      <c r="DX3" s="43"/>
-      <c r="DY3" s="46" t="s">
+      <c r="DR3" s="46"/>
+      <c r="DS3" s="46"/>
+      <c r="DT3" s="46"/>
+      <c r="DU3" s="46"/>
+      <c r="DV3" s="46"/>
+      <c r="DW3" s="46"/>
+      <c r="DX3" s="47"/>
+      <c r="DY3" s="49" t="s">
         <v>7</v>
       </c>
       <c r="DZ3" s="18"/>
@@ -5171,7 +5200,7 @@
       <c r="DV9" s="17"/>
       <c r="DW9" s="17"/>
       <c r="DX9" s="22"/>
-      <c r="DZ9" s="44" t="s">
+      <c r="DZ9" s="48" t="s">
         <v>14</v>
       </c>
       <c r="EA9" s="28" t="s">
@@ -5346,7 +5375,7 @@
       <c r="DV10" s="17"/>
       <c r="DW10" s="17"/>
       <c r="DX10" s="22"/>
-      <c r="DZ10" s="44" t="s">
+      <c r="DZ10" s="48" t="s">
         <v>20</v>
       </c>
       <c r="EA10" s="28"/>
@@ -5515,7 +5544,7 @@
       <c r="DV11" s="17"/>
       <c r="DW11" s="17"/>
       <c r="DX11" s="22"/>
-      <c r="DZ11" s="44" t="s">
+      <c r="DZ11" s="48" t="s">
         <v>24</v>
       </c>
       <c r="EA11" s="28"/>
@@ -5682,7 +5711,7 @@
       <c r="DV12" s="17"/>
       <c r="DW12" s="17"/>
       <c r="DX12" s="22"/>
-      <c r="DZ12" s="44" t="s">
+      <c r="DZ12" s="48" t="s">
         <v>26</v>
       </c>
       <c r="EA12" s="28"/>
@@ -5849,7 +5878,7 @@
       <c r="DV13" s="17"/>
       <c r="DW13" s="17"/>
       <c r="DX13" s="22"/>
-      <c r="DZ13" s="44" t="s">
+      <c r="DZ13" s="48" t="s">
         <v>27</v>
       </c>
       <c r="EA13" s="28"/>
@@ -6012,7 +6041,7 @@
       <c r="DV14" s="7"/>
       <c r="DW14" s="7"/>
       <c r="DX14" s="32"/>
-      <c r="DZ14" s="44" t="s">
+      <c r="DZ14" s="48" t="s">
         <v>28</v>
       </c>
       <c r="EA14" s="28"/>
@@ -6113,7 +6142,7 @@
       <c r="CP15" s="17"/>
       <c r="CQ15" s="17"/>
       <c r="CR15" s="22"/>
-      <c r="DZ15" s="45" t="s">
+      <c r="DZ15" s="8" t="s">
         <v>29</v>
       </c>
       <c r="EA15" s="28"/>
@@ -6272,7 +6301,7 @@
       <c r="DV16" s="3"/>
       <c r="DW16" s="3"/>
       <c r="DX16" s="21"/>
-      <c r="DZ16" s="45"/>
+      <c r="DZ16" s="8"/>
       <c r="EA16" s="28"/>
       <c r="EB16" s="28"/>
       <c r="EC16" s="28"/>
@@ -6402,38 +6431,38 @@
       <c r="CP17" s="17"/>
       <c r="CQ17" s="17"/>
       <c r="CR17" s="22"/>
-      <c r="CT17" s="4"/>
-      <c r="CU17" s="5"/>
-      <c r="CV17" s="5"/>
-      <c r="CW17" s="5"/>
-      <c r="CX17" s="5"/>
-      <c r="CY17" s="5"/>
-      <c r="CZ17" s="5"/>
-      <c r="DA17" s="5"/>
-      <c r="DB17" s="5"/>
-      <c r="DC17" s="5"/>
-      <c r="DD17" s="5"/>
-      <c r="DE17" s="5"/>
-      <c r="DF17" s="5"/>
-      <c r="DG17" s="5"/>
-      <c r="DH17" s="5"/>
-      <c r="DI17" s="5"/>
-      <c r="DJ17" s="5"/>
-      <c r="DK17" s="5"/>
-      <c r="DL17" s="5"/>
-      <c r="DM17" s="5"/>
-      <c r="DN17" s="5"/>
-      <c r="DO17" s="5"/>
-      <c r="DP17" s="5"/>
-      <c r="DQ17" s="5"/>
-      <c r="DR17" s="5"/>
-      <c r="DS17" s="5"/>
-      <c r="DT17" s="5"/>
-      <c r="DU17" s="5"/>
-      <c r="DV17" s="5"/>
-      <c r="DW17" s="5"/>
+      <c r="CT17" s="38"/>
+      <c r="CU17" s="39"/>
+      <c r="CV17" s="39"/>
+      <c r="CW17" s="39"/>
+      <c r="CX17" s="39"/>
+      <c r="CY17" s="39"/>
+      <c r="CZ17" s="39"/>
+      <c r="DA17" s="39"/>
+      <c r="DB17" s="39"/>
+      <c r="DC17" s="39"/>
+      <c r="DD17" s="39"/>
+      <c r="DE17" s="39"/>
+      <c r="DF17" s="39"/>
+      <c r="DG17" s="39"/>
+      <c r="DH17" s="39"/>
+      <c r="DI17" s="39"/>
+      <c r="DJ17" s="39"/>
+      <c r="DK17" s="39"/>
+      <c r="DL17" s="39"/>
+      <c r="DM17" s="39"/>
+      <c r="DN17" s="39"/>
+      <c r="DO17" s="39"/>
+      <c r="DP17" s="39"/>
+      <c r="DQ17" s="39"/>
+      <c r="DR17" s="39"/>
+      <c r="DS17" s="39"/>
+      <c r="DT17" s="39"/>
+      <c r="DU17" s="39"/>
+      <c r="DV17" s="39"/>
+      <c r="DW17" s="39"/>
       <c r="DX17" s="22"/>
-      <c r="DZ17" s="44" t="s">
+      <c r="DZ17" s="48" t="s">
         <v>30</v>
       </c>
       <c r="EA17" s="28"/>
@@ -6504,37 +6533,37 @@
       <c r="AH18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="AI18" s="29" t="s">
+      <c r="AI18" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="AJ18" s="29"/>
-      <c r="AK18" s="29"/>
-      <c r="AL18" s="29"/>
-      <c r="AM18" s="29"/>
-      <c r="AN18" s="29"/>
-      <c r="AO18" s="29"/>
-      <c r="AP18" s="29"/>
-      <c r="AQ18" s="29"/>
-      <c r="AR18" s="29"/>
-      <c r="AS18" s="29"/>
-      <c r="AT18" s="29"/>
-      <c r="AU18" s="29"/>
-      <c r="AV18" s="29"/>
-      <c r="AW18" s="29"/>
-      <c r="AX18" s="29"/>
-      <c r="AY18" s="29"/>
-      <c r="AZ18" s="29"/>
-      <c r="BA18" s="29"/>
-      <c r="BB18" s="29"/>
-      <c r="BC18" s="29"/>
-      <c r="BD18" s="29"/>
-      <c r="BE18" s="29"/>
-      <c r="BF18" s="29"/>
-      <c r="BG18" s="29"/>
-      <c r="BH18" s="29"/>
-      <c r="BI18" s="29"/>
-      <c r="BJ18" s="29"/>
-      <c r="BK18" s="29"/>
+      <c r="AJ18" s="17"/>
+      <c r="AK18" s="17"/>
+      <c r="AL18" s="17"/>
+      <c r="AM18" s="17"/>
+      <c r="AN18" s="17"/>
+      <c r="AO18" s="17"/>
+      <c r="AP18" s="17"/>
+      <c r="AQ18" s="17"/>
+      <c r="AR18" s="17"/>
+      <c r="AS18" s="17"/>
+      <c r="AT18" s="17"/>
+      <c r="AU18" s="17"/>
+      <c r="AV18" s="17"/>
+      <c r="AW18" s="17"/>
+      <c r="AX18" s="17"/>
+      <c r="AY18" s="17"/>
+      <c r="AZ18" s="17"/>
+      <c r="BA18" s="17"/>
+      <c r="BB18" s="17"/>
+      <c r="BC18" s="17"/>
+      <c r="BD18" s="17"/>
+      <c r="BE18" s="17"/>
+      <c r="BF18" s="17"/>
+      <c r="BG18" s="17"/>
+      <c r="BH18" s="17"/>
+      <c r="BI18" s="17"/>
+      <c r="BJ18" s="17"/>
+      <c r="BK18" s="17"/>
       <c r="BL18" s="22"/>
       <c r="BN18" s="8" t="s">
         <v>31</v>
@@ -6604,7 +6633,7 @@
       <c r="DV18" s="17"/>
       <c r="DW18" s="17"/>
       <c r="DX18" s="22"/>
-      <c r="DZ18" s="44" t="s">
+      <c r="DZ18" s="48" t="s">
         <v>31</v>
       </c>
       <c r="EA18" s="28"/>
@@ -6675,37 +6704,37 @@
       <c r="AH19" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="AI19" s="29" t="s">
+      <c r="AI19" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="AJ19" s="29"/>
-      <c r="AK19" s="29"/>
-      <c r="AL19" s="29"/>
-      <c r="AM19" s="29"/>
-      <c r="AN19" s="29"/>
-      <c r="AO19" s="29"/>
-      <c r="AP19" s="29"/>
-      <c r="AQ19" s="29"/>
-      <c r="AR19" s="29"/>
-      <c r="AS19" s="29"/>
-      <c r="AT19" s="29"/>
-      <c r="AU19" s="29"/>
-      <c r="AV19" s="29"/>
-      <c r="AW19" s="29"/>
-      <c r="AX19" s="29"/>
-      <c r="AY19" s="29"/>
-      <c r="AZ19" s="29"/>
-      <c r="BA19" s="29"/>
-      <c r="BB19" s="29"/>
-      <c r="BC19" s="29"/>
-      <c r="BD19" s="29"/>
-      <c r="BE19" s="29"/>
-      <c r="BF19" s="29"/>
-      <c r="BG19" s="29"/>
-      <c r="BH19" s="29"/>
-      <c r="BI19" s="29"/>
-      <c r="BJ19" s="29"/>
-      <c r="BK19" s="29"/>
+      <c r="AJ19" s="17"/>
+      <c r="AK19" s="17"/>
+      <c r="AL19" s="17"/>
+      <c r="AM19" s="17"/>
+      <c r="AN19" s="17"/>
+      <c r="AO19" s="17"/>
+      <c r="AP19" s="17"/>
+      <c r="AQ19" s="17"/>
+      <c r="AR19" s="17"/>
+      <c r="AS19" s="17"/>
+      <c r="AT19" s="17"/>
+      <c r="AU19" s="17"/>
+      <c r="AV19" s="17"/>
+      <c r="AW19" s="17"/>
+      <c r="AX19" s="17"/>
+      <c r="AY19" s="17"/>
+      <c r="AZ19" s="17"/>
+      <c r="BA19" s="17"/>
+      <c r="BB19" s="17"/>
+      <c r="BC19" s="17"/>
+      <c r="BD19" s="17"/>
+      <c r="BE19" s="17"/>
+      <c r="BF19" s="17"/>
+      <c r="BG19" s="17"/>
+      <c r="BH19" s="17"/>
+      <c r="BI19" s="17"/>
+      <c r="BJ19" s="17"/>
+      <c r="BK19" s="17"/>
       <c r="BL19" s="22"/>
       <c r="BN19" s="8" t="s">
         <v>34</v>
@@ -6743,39 +6772,39 @@
       <c r="CT19" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="CU19" s="17" t="s">
+      <c r="CU19" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="CV19" s="17"/>
-      <c r="CW19" s="17"/>
-      <c r="CX19" s="17"/>
-      <c r="CY19" s="17"/>
-      <c r="CZ19" s="17"/>
-      <c r="DA19" s="17"/>
-      <c r="DB19" s="17"/>
-      <c r="DC19" s="17"/>
-      <c r="DD19" s="17"/>
-      <c r="DE19" s="17"/>
-      <c r="DF19" s="17"/>
-      <c r="DG19" s="17"/>
-      <c r="DH19" s="17"/>
-      <c r="DI19" s="17"/>
-      <c r="DJ19" s="17"/>
-      <c r="DK19" s="17"/>
-      <c r="DL19" s="17"/>
-      <c r="DM19" s="17"/>
-      <c r="DN19" s="17"/>
-      <c r="DO19" s="17"/>
-      <c r="DP19" s="17"/>
-      <c r="DQ19" s="17"/>
-      <c r="DR19" s="17"/>
-      <c r="DS19" s="17"/>
-      <c r="DT19" s="17"/>
-      <c r="DU19" s="17"/>
-      <c r="DV19" s="17"/>
-      <c r="DW19" s="17"/>
+      <c r="CV19" s="41"/>
+      <c r="CW19" s="41"/>
+      <c r="CX19" s="41"/>
+      <c r="CY19" s="41"/>
+      <c r="CZ19" s="41"/>
+      <c r="DA19" s="41"/>
+      <c r="DB19" s="41"/>
+      <c r="DC19" s="41"/>
+      <c r="DD19" s="41"/>
+      <c r="DE19" s="41"/>
+      <c r="DF19" s="41"/>
+      <c r="DG19" s="41"/>
+      <c r="DH19" s="41"/>
+      <c r="DI19" s="41"/>
+      <c r="DJ19" s="41"/>
+      <c r="DK19" s="41"/>
+      <c r="DL19" s="41"/>
+      <c r="DM19" s="41"/>
+      <c r="DN19" s="41"/>
+      <c r="DO19" s="41"/>
+      <c r="DP19" s="41"/>
+      <c r="DQ19" s="41"/>
+      <c r="DR19" s="41"/>
+      <c r="DS19" s="41"/>
+      <c r="DT19" s="41"/>
+      <c r="DU19" s="41"/>
+      <c r="DV19" s="41"/>
+      <c r="DW19" s="41"/>
       <c r="DX19" s="22"/>
-      <c r="DZ19" s="44" t="s">
+      <c r="DZ19" s="48" t="s">
         <v>34</v>
       </c>
       <c r="EA19" s="28"/>
@@ -6846,37 +6875,37 @@
       <c r="AH20" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="AI20" s="29" t="s">
+      <c r="AI20" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="AJ20" s="29"/>
-      <c r="AK20" s="29"/>
-      <c r="AL20" s="29"/>
-      <c r="AM20" s="29"/>
-      <c r="AN20" s="29"/>
-      <c r="AO20" s="29"/>
-      <c r="AP20" s="29"/>
-      <c r="AQ20" s="29"/>
-      <c r="AR20" s="29"/>
-      <c r="AS20" s="29"/>
-      <c r="AT20" s="29"/>
-      <c r="AU20" s="29"/>
-      <c r="AV20" s="29"/>
-      <c r="AW20" s="29"/>
-      <c r="AX20" s="29"/>
-      <c r="AY20" s="29"/>
-      <c r="AZ20" s="29"/>
-      <c r="BA20" s="29"/>
-      <c r="BB20" s="29"/>
-      <c r="BC20" s="29"/>
-      <c r="BD20" s="29"/>
-      <c r="BE20" s="29"/>
-      <c r="BF20" s="29"/>
-      <c r="BG20" s="29"/>
-      <c r="BH20" s="29"/>
-      <c r="BI20" s="29"/>
-      <c r="BJ20" s="29"/>
-      <c r="BK20" s="29"/>
+      <c r="AJ20" s="17"/>
+      <c r="AK20" s="17"/>
+      <c r="AL20" s="17"/>
+      <c r="AM20" s="17"/>
+      <c r="AN20" s="17"/>
+      <c r="AO20" s="17"/>
+      <c r="AP20" s="17"/>
+      <c r="AQ20" s="17"/>
+      <c r="AR20" s="17"/>
+      <c r="AS20" s="17"/>
+      <c r="AT20" s="17"/>
+      <c r="AU20" s="17"/>
+      <c r="AV20" s="17"/>
+      <c r="AW20" s="17"/>
+      <c r="AX20" s="17"/>
+      <c r="AY20" s="17"/>
+      <c r="AZ20" s="17"/>
+      <c r="BA20" s="17"/>
+      <c r="BB20" s="17"/>
+      <c r="BC20" s="17"/>
+      <c r="BD20" s="17"/>
+      <c r="BE20" s="17"/>
+      <c r="BF20" s="17"/>
+      <c r="BG20" s="17"/>
+      <c r="BH20" s="17"/>
+      <c r="BI20" s="17"/>
+      <c r="BJ20" s="17"/>
+      <c r="BK20" s="17"/>
       <c r="BL20" s="22"/>
       <c r="BN20" s="8" t="s">
         <v>37</v>
@@ -6944,7 +6973,7 @@
       <c r="DV20" s="17"/>
       <c r="DW20" s="17"/>
       <c r="DX20" s="22"/>
-      <c r="DZ20" s="44" t="s">
+      <c r="DZ20" s="48" t="s">
         <v>37</v>
       </c>
       <c r="EA20" s="28"/>
@@ -7015,37 +7044,37 @@
       <c r="AH21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AI21" s="29" t="s">
+      <c r="AI21" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="AJ21" s="29"/>
-      <c r="AK21" s="29"/>
-      <c r="AL21" s="29"/>
-      <c r="AM21" s="29"/>
-      <c r="AN21" s="29"/>
-      <c r="AO21" s="29"/>
-      <c r="AP21" s="29"/>
-      <c r="AQ21" s="29"/>
-      <c r="AR21" s="29"/>
-      <c r="AS21" s="29"/>
-      <c r="AT21" s="29"/>
-      <c r="AU21" s="29"/>
-      <c r="AV21" s="29"/>
-      <c r="AW21" s="29"/>
-      <c r="AX21" s="29"/>
-      <c r="AY21" s="29"/>
-      <c r="AZ21" s="29"/>
-      <c r="BA21" s="29"/>
-      <c r="BB21" s="29"/>
-      <c r="BC21" s="29"/>
-      <c r="BD21" s="29"/>
-      <c r="BE21" s="29"/>
-      <c r="BF21" s="29"/>
-      <c r="BG21" s="29"/>
-      <c r="BH21" s="29"/>
-      <c r="BI21" s="29"/>
-      <c r="BJ21" s="29"/>
-      <c r="BK21" s="29"/>
+      <c r="AJ21" s="17"/>
+      <c r="AK21" s="17"/>
+      <c r="AL21" s="17"/>
+      <c r="AM21" s="17"/>
+      <c r="AN21" s="17"/>
+      <c r="AO21" s="17"/>
+      <c r="AP21" s="17"/>
+      <c r="AQ21" s="17"/>
+      <c r="AR21" s="17"/>
+      <c r="AS21" s="17"/>
+      <c r="AT21" s="17"/>
+      <c r="AU21" s="17"/>
+      <c r="AV21" s="17"/>
+      <c r="AW21" s="17"/>
+      <c r="AX21" s="17"/>
+      <c r="AY21" s="17"/>
+      <c r="AZ21" s="17"/>
+      <c r="BA21" s="17"/>
+      <c r="BB21" s="17"/>
+      <c r="BC21" s="17"/>
+      <c r="BD21" s="17"/>
+      <c r="BE21" s="17"/>
+      <c r="BF21" s="17"/>
+      <c r="BG21" s="17"/>
+      <c r="BH21" s="17"/>
+      <c r="BI21" s="17"/>
+      <c r="BJ21" s="17"/>
+      <c r="BK21" s="17"/>
       <c r="BL21" s="22"/>
       <c r="BN21" s="8" t="s">
         <v>39</v>
@@ -7113,7 +7142,7 @@
       <c r="DV21" s="17"/>
       <c r="DW21" s="17"/>
       <c r="DX21" s="22"/>
-      <c r="DZ21" s="44" t="s">
+      <c r="DZ21" s="48" t="s">
         <v>39</v>
       </c>
       <c r="EA21" s="28"/>
@@ -7184,35 +7213,35 @@
       <c r="AH22" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AI22" s="29"/>
-      <c r="AJ22" s="29"/>
-      <c r="AK22" s="29"/>
-      <c r="AL22" s="29"/>
-      <c r="AM22" s="29"/>
-      <c r="AN22" s="29"/>
-      <c r="AO22" s="29"/>
-      <c r="AP22" s="29"/>
-      <c r="AQ22" s="29"/>
-      <c r="AR22" s="29"/>
-      <c r="AS22" s="29"/>
-      <c r="AT22" s="29"/>
-      <c r="AU22" s="29"/>
-      <c r="AV22" s="29"/>
-      <c r="AW22" s="29"/>
-      <c r="AX22" s="29"/>
-      <c r="AY22" s="29"/>
-      <c r="AZ22" s="29"/>
-      <c r="BA22" s="29"/>
-      <c r="BB22" s="29"/>
-      <c r="BC22" s="29"/>
-      <c r="BD22" s="29"/>
-      <c r="BE22" s="29"/>
-      <c r="BF22" s="29"/>
-      <c r="BG22" s="29"/>
-      <c r="BH22" s="29"/>
-      <c r="BI22" s="29"/>
-      <c r="BJ22" s="29"/>
-      <c r="BK22" s="29"/>
+      <c r="AI22" s="17"/>
+      <c r="AJ22" s="17"/>
+      <c r="AK22" s="17"/>
+      <c r="AL22" s="17"/>
+      <c r="AM22" s="17"/>
+      <c r="AN22" s="17"/>
+      <c r="AO22" s="17"/>
+      <c r="AP22" s="17"/>
+      <c r="AQ22" s="17"/>
+      <c r="AR22" s="17"/>
+      <c r="AS22" s="17"/>
+      <c r="AT22" s="17"/>
+      <c r="AU22" s="17"/>
+      <c r="AV22" s="17"/>
+      <c r="AW22" s="17"/>
+      <c r="AX22" s="17"/>
+      <c r="AY22" s="17"/>
+      <c r="AZ22" s="17"/>
+      <c r="BA22" s="17"/>
+      <c r="BB22" s="17"/>
+      <c r="BC22" s="17"/>
+      <c r="BD22" s="17"/>
+      <c r="BE22" s="17"/>
+      <c r="BF22" s="17"/>
+      <c r="BG22" s="17"/>
+      <c r="BH22" s="17"/>
+      <c r="BI22" s="17"/>
+      <c r="BJ22" s="17"/>
+      <c r="BK22" s="17"/>
       <c r="BL22" s="22"/>
       <c r="BN22" s="8" t="s">
         <v>41</v>
@@ -7280,7 +7309,7 @@
       <c r="DV22" s="17"/>
       <c r="DW22" s="17"/>
       <c r="DX22" s="22"/>
-      <c r="DZ22" s="44" t="s">
+      <c r="DZ22" s="48" t="s">
         <v>41</v>
       </c>
       <c r="EA22" s="28"/>
@@ -7351,35 +7380,35 @@
       <c r="AH23" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AI23" s="29"/>
-      <c r="AJ23" s="29"/>
-      <c r="AK23" s="29"/>
-      <c r="AL23" s="29"/>
-      <c r="AM23" s="29"/>
-      <c r="AN23" s="29"/>
-      <c r="AO23" s="29"/>
-      <c r="AP23" s="29"/>
-      <c r="AQ23" s="29"/>
-      <c r="AR23" s="29"/>
-      <c r="AS23" s="29"/>
-      <c r="AT23" s="29"/>
-      <c r="AU23" s="29"/>
-      <c r="AV23" s="29"/>
-      <c r="AW23" s="29"/>
-      <c r="AX23" s="29"/>
-      <c r="AY23" s="29"/>
-      <c r="AZ23" s="29"/>
-      <c r="BA23" s="29"/>
-      <c r="BB23" s="29"/>
-      <c r="BC23" s="29"/>
-      <c r="BD23" s="29"/>
-      <c r="BE23" s="29"/>
-      <c r="BF23" s="29"/>
-      <c r="BG23" s="29"/>
-      <c r="BH23" s="29"/>
-      <c r="BI23" s="29"/>
-      <c r="BJ23" s="29"/>
-      <c r="BK23" s="29"/>
+      <c r="AI23" s="17"/>
+      <c r="AJ23" s="17"/>
+      <c r="AK23" s="17"/>
+      <c r="AL23" s="17"/>
+      <c r="AM23" s="17"/>
+      <c r="AN23" s="17"/>
+      <c r="AO23" s="17"/>
+      <c r="AP23" s="17"/>
+      <c r="AQ23" s="17"/>
+      <c r="AR23" s="17"/>
+      <c r="AS23" s="17"/>
+      <c r="AT23" s="17"/>
+      <c r="AU23" s="17"/>
+      <c r="AV23" s="17"/>
+      <c r="AW23" s="17"/>
+      <c r="AX23" s="17"/>
+      <c r="AY23" s="17"/>
+      <c r="AZ23" s="17"/>
+      <c r="BA23" s="17"/>
+      <c r="BB23" s="17"/>
+      <c r="BC23" s="17"/>
+      <c r="BD23" s="17"/>
+      <c r="BE23" s="17"/>
+      <c r="BF23" s="17"/>
+      <c r="BG23" s="17"/>
+      <c r="BH23" s="17"/>
+      <c r="BI23" s="17"/>
+      <c r="BJ23" s="17"/>
+      <c r="BK23" s="17"/>
       <c r="BL23" s="22"/>
       <c r="BN23" s="8" t="s">
         <v>42</v>
@@ -7447,7 +7476,7 @@
       <c r="DV23" s="17"/>
       <c r="DW23" s="17"/>
       <c r="DX23" s="22"/>
-      <c r="DZ23" s="44" t="s">
+      <c r="DZ23" s="48" t="s">
         <v>42</v>
       </c>
       <c r="EA23" s="28"/>
@@ -8038,47 +8067,47 @@
       <c r="AL28" s="17"/>
       <c r="AM28" s="17"/>
       <c r="AN28" s="17"/>
-      <c r="AO28" s="30">
+      <c r="AO28" s="29">
         <v>8</v>
       </c>
-      <c r="AP28" s="17"/>
-      <c r="AQ28" s="17"/>
-      <c r="AR28" s="17"/>
-      <c r="AS28" s="17"/>
-      <c r="AT28" s="17"/>
-      <c r="AU28" s="17"/>
-      <c r="AV28" s="17"/>
-      <c r="AW28" s="17"/>
-      <c r="AX28" s="17"/>
-      <c r="AY28" s="17"/>
-      <c r="AZ28" s="17"/>
-      <c r="BA28" s="17"/>
-      <c r="BB28" s="17"/>
-      <c r="BC28" s="17"/>
-      <c r="BD28" s="17"/>
-      <c r="BE28" s="17"/>
-      <c r="BF28" s="17"/>
-      <c r="BG28" s="17"/>
-      <c r="BH28" s="17"/>
-      <c r="BI28" s="17"/>
-      <c r="BJ28" s="17"/>
-      <c r="BK28" s="17"/>
-      <c r="BL28" s="17"/>
-      <c r="BM28" s="17"/>
-      <c r="BN28" s="17"/>
-      <c r="BO28" s="17"/>
-      <c r="BP28" s="17"/>
-      <c r="BQ28" s="17"/>
-      <c r="BR28" s="17"/>
-      <c r="BS28" s="17"/>
-      <c r="BT28" s="17"/>
-      <c r="BU28" s="17"/>
-      <c r="BV28" s="17"/>
-      <c r="BW28" s="17"/>
-      <c r="BX28" s="17"/>
-      <c r="BY28" s="17"/>
-      <c r="BZ28" s="17"/>
-      <c r="CA28" s="17"/>
+      <c r="AP28" s="30"/>
+      <c r="AQ28" s="30"/>
+      <c r="AR28" s="30"/>
+      <c r="AS28" s="30"/>
+      <c r="AT28" s="30"/>
+      <c r="AU28" s="30"/>
+      <c r="AV28" s="30"/>
+      <c r="AW28" s="30"/>
+      <c r="AX28" s="30"/>
+      <c r="AY28" s="30"/>
+      <c r="AZ28" s="30"/>
+      <c r="BA28" s="30"/>
+      <c r="BB28" s="30"/>
+      <c r="BC28" s="30"/>
+      <c r="BD28" s="30"/>
+      <c r="BE28" s="30"/>
+      <c r="BF28" s="30"/>
+      <c r="BG28" s="30"/>
+      <c r="BH28" s="30"/>
+      <c r="BI28" s="30"/>
+      <c r="BJ28" s="30"/>
+      <c r="BK28" s="30"/>
+      <c r="BL28" s="30"/>
+      <c r="BM28" s="30"/>
+      <c r="BN28" s="30"/>
+      <c r="BO28" s="30"/>
+      <c r="BP28" s="30"/>
+      <c r="BQ28" s="30"/>
+      <c r="BR28" s="30"/>
+      <c r="BS28" s="30"/>
+      <c r="BT28" s="30"/>
+      <c r="BU28" s="30"/>
+      <c r="BV28" s="30"/>
+      <c r="BW28" s="30"/>
+      <c r="BX28" s="30"/>
+      <c r="BY28" s="30"/>
+      <c r="BZ28" s="30"/>
+      <c r="CA28" s="30"/>
       <c r="CB28" s="5"/>
       <c r="CC28" s="22"/>
       <c r="CD28" s="33"/>
@@ -8125,46 +8154,46 @@
       <c r="DO28" s="17"/>
       <c r="DP28" s="17"/>
       <c r="DQ28" s="17"/>
-      <c r="DR28" s="30">
+      <c r="DR28" s="29">
         <v>8</v>
       </c>
-      <c r="DS28" s="17"/>
-      <c r="DT28" s="17"/>
-      <c r="DU28" s="17"/>
-      <c r="DV28" s="17"/>
-      <c r="DW28" s="17"/>
-      <c r="DX28" s="17"/>
-      <c r="DY28" s="17"/>
-      <c r="DZ28" s="17"/>
-      <c r="EA28" s="17"/>
-      <c r="EB28" s="17"/>
-      <c r="EC28" s="17"/>
-      <c r="ED28" s="17"/>
-      <c r="EE28" s="17"/>
-      <c r="EF28" s="17"/>
-      <c r="EG28" s="17"/>
-      <c r="EH28" s="17"/>
-      <c r="EI28" s="17"/>
-      <c r="EJ28" s="17"/>
-      <c r="EK28" s="17"/>
-      <c r="EL28" s="17"/>
-      <c r="EM28" s="17"/>
-      <c r="EN28" s="17"/>
-      <c r="EO28" s="17"/>
-      <c r="EP28" s="17"/>
-      <c r="EQ28" s="17"/>
-      <c r="ER28" s="17"/>
-      <c r="ES28" s="17"/>
-      <c r="ET28" s="17"/>
-      <c r="EU28" s="17"/>
-      <c r="EV28" s="17"/>
-      <c r="EW28" s="17"/>
-      <c r="EX28" s="17"/>
-      <c r="EY28" s="17"/>
-      <c r="EZ28" s="17"/>
-      <c r="FA28" s="17"/>
-      <c r="FB28" s="17"/>
-      <c r="FC28" s="17"/>
+      <c r="DS28" s="30"/>
+      <c r="DT28" s="30"/>
+      <c r="DU28" s="30"/>
+      <c r="DV28" s="30"/>
+      <c r="DW28" s="30"/>
+      <c r="DX28" s="30"/>
+      <c r="DY28" s="30"/>
+      <c r="DZ28" s="30"/>
+      <c r="EA28" s="30"/>
+      <c r="EB28" s="30"/>
+      <c r="EC28" s="30"/>
+      <c r="ED28" s="30"/>
+      <c r="EE28" s="30"/>
+      <c r="EF28" s="30"/>
+      <c r="EG28" s="30"/>
+      <c r="EH28" s="30"/>
+      <c r="EI28" s="30"/>
+      <c r="EJ28" s="30"/>
+      <c r="EK28" s="30"/>
+      <c r="EL28" s="30"/>
+      <c r="EM28" s="30"/>
+      <c r="EN28" s="30"/>
+      <c r="EO28" s="30"/>
+      <c r="EP28" s="30"/>
+      <c r="EQ28" s="30"/>
+      <c r="ER28" s="30"/>
+      <c r="ES28" s="30"/>
+      <c r="ET28" s="30"/>
+      <c r="EU28" s="30"/>
+      <c r="EV28" s="30"/>
+      <c r="EW28" s="30"/>
+      <c r="EX28" s="30"/>
+      <c r="EY28" s="30"/>
+      <c r="EZ28" s="30"/>
+      <c r="FA28" s="30"/>
+      <c r="FB28" s="30"/>
+      <c r="FC28" s="30"/>
       <c r="FD28" s="24"/>
     </row>
     <row r="29" customHeight="1" spans="2:160">
@@ -8211,47 +8240,47 @@
       <c r="AL29" s="17"/>
       <c r="AM29" s="17"/>
       <c r="AN29" s="17"/>
-      <c r="AO29" s="30">
+      <c r="AO29" s="29">
         <v>9</v>
       </c>
-      <c r="AP29" s="17"/>
-      <c r="AQ29" s="17"/>
-      <c r="AR29" s="17"/>
-      <c r="AS29" s="17"/>
-      <c r="AT29" s="17"/>
-      <c r="AU29" s="17"/>
-      <c r="AV29" s="17"/>
-      <c r="AW29" s="17"/>
-      <c r="AX29" s="17"/>
-      <c r="AY29" s="17"/>
-      <c r="AZ29" s="17"/>
-      <c r="BA29" s="17"/>
-      <c r="BB29" s="17"/>
-      <c r="BC29" s="17"/>
-      <c r="BD29" s="17"/>
-      <c r="BE29" s="17"/>
-      <c r="BF29" s="17"/>
-      <c r="BG29" s="17"/>
-      <c r="BH29" s="17"/>
-      <c r="BI29" s="17"/>
-      <c r="BJ29" s="17"/>
-      <c r="BK29" s="17"/>
-      <c r="BL29" s="17"/>
-      <c r="BM29" s="17"/>
-      <c r="BN29" s="17"/>
-      <c r="BO29" s="17"/>
-      <c r="BP29" s="17"/>
-      <c r="BQ29" s="17"/>
-      <c r="BR29" s="17"/>
-      <c r="BS29" s="17"/>
-      <c r="BT29" s="17"/>
-      <c r="BU29" s="17"/>
-      <c r="BV29" s="17"/>
-      <c r="BW29" s="17"/>
-      <c r="BX29" s="17"/>
-      <c r="BY29" s="17"/>
-      <c r="BZ29" s="17"/>
-      <c r="CA29" s="17"/>
+      <c r="AP29" s="30"/>
+      <c r="AQ29" s="30"/>
+      <c r="AR29" s="30"/>
+      <c r="AS29" s="30"/>
+      <c r="AT29" s="30"/>
+      <c r="AU29" s="30"/>
+      <c r="AV29" s="30"/>
+      <c r="AW29" s="30"/>
+      <c r="AX29" s="30"/>
+      <c r="AY29" s="30"/>
+      <c r="AZ29" s="30"/>
+      <c r="BA29" s="30"/>
+      <c r="BB29" s="30"/>
+      <c r="BC29" s="30"/>
+      <c r="BD29" s="30"/>
+      <c r="BE29" s="30"/>
+      <c r="BF29" s="30"/>
+      <c r="BG29" s="30"/>
+      <c r="BH29" s="30"/>
+      <c r="BI29" s="30"/>
+      <c r="BJ29" s="30"/>
+      <c r="BK29" s="30"/>
+      <c r="BL29" s="30"/>
+      <c r="BM29" s="30"/>
+      <c r="BN29" s="30"/>
+      <c r="BO29" s="30"/>
+      <c r="BP29" s="30"/>
+      <c r="BQ29" s="30"/>
+      <c r="BR29" s="30"/>
+      <c r="BS29" s="30"/>
+      <c r="BT29" s="30"/>
+      <c r="BU29" s="30"/>
+      <c r="BV29" s="30"/>
+      <c r="BW29" s="30"/>
+      <c r="BX29" s="30"/>
+      <c r="BY29" s="30"/>
+      <c r="BZ29" s="30"/>
+      <c r="CA29" s="30"/>
       <c r="CB29" s="5"/>
       <c r="CC29" s="22"/>
       <c r="CD29" s="33"/>
@@ -8298,46 +8327,46 @@
       <c r="DO29" s="17"/>
       <c r="DP29" s="17"/>
       <c r="DQ29" s="17"/>
-      <c r="DR29" s="30">
+      <c r="DR29" s="29">
         <v>9</v>
       </c>
-      <c r="DS29" s="17"/>
-      <c r="DT29" s="17"/>
-      <c r="DU29" s="17"/>
-      <c r="DV29" s="17"/>
-      <c r="DW29" s="17"/>
-      <c r="DX29" s="17"/>
-      <c r="DY29" s="17"/>
-      <c r="DZ29" s="17"/>
-      <c r="EA29" s="17"/>
-      <c r="EB29" s="17"/>
-      <c r="EC29" s="17"/>
-      <c r="ED29" s="17"/>
-      <c r="EE29" s="17"/>
-      <c r="EF29" s="17"/>
-      <c r="EG29" s="17"/>
-      <c r="EH29" s="17"/>
-      <c r="EI29" s="17"/>
-      <c r="EJ29" s="17"/>
-      <c r="EK29" s="17"/>
-      <c r="EL29" s="17"/>
-      <c r="EM29" s="17"/>
-      <c r="EN29" s="17"/>
-      <c r="EO29" s="17"/>
-      <c r="EP29" s="17"/>
-      <c r="EQ29" s="17"/>
-      <c r="ER29" s="17"/>
-      <c r="ES29" s="17"/>
-      <c r="ET29" s="17"/>
-      <c r="EU29" s="17"/>
-      <c r="EV29" s="17"/>
-      <c r="EW29" s="17"/>
-      <c r="EX29" s="17"/>
-      <c r="EY29" s="17"/>
-      <c r="EZ29" s="17"/>
-      <c r="FA29" s="17"/>
-      <c r="FB29" s="17"/>
-      <c r="FC29" s="17"/>
+      <c r="DS29" s="30"/>
+      <c r="DT29" s="30"/>
+      <c r="DU29" s="30"/>
+      <c r="DV29" s="30"/>
+      <c r="DW29" s="30"/>
+      <c r="DX29" s="30"/>
+      <c r="DY29" s="30"/>
+      <c r="DZ29" s="30"/>
+      <c r="EA29" s="30"/>
+      <c r="EB29" s="30"/>
+      <c r="EC29" s="30"/>
+      <c r="ED29" s="30"/>
+      <c r="EE29" s="30"/>
+      <c r="EF29" s="30"/>
+      <c r="EG29" s="30"/>
+      <c r="EH29" s="30"/>
+      <c r="EI29" s="30"/>
+      <c r="EJ29" s="30"/>
+      <c r="EK29" s="30"/>
+      <c r="EL29" s="30"/>
+      <c r="EM29" s="30"/>
+      <c r="EN29" s="30"/>
+      <c r="EO29" s="30"/>
+      <c r="EP29" s="30"/>
+      <c r="EQ29" s="30"/>
+      <c r="ER29" s="30"/>
+      <c r="ES29" s="30"/>
+      <c r="ET29" s="30"/>
+      <c r="EU29" s="30"/>
+      <c r="EV29" s="30"/>
+      <c r="EW29" s="30"/>
+      <c r="EX29" s="30"/>
+      <c r="EY29" s="30"/>
+      <c r="EZ29" s="30"/>
+      <c r="FA29" s="30"/>
+      <c r="FB29" s="30"/>
+      <c r="FC29" s="30"/>
       <c r="FD29" s="24"/>
     </row>
     <row r="30" customHeight="1" spans="2:160">
@@ -8384,47 +8413,47 @@
       <c r="AL30" s="17"/>
       <c r="AM30" s="17"/>
       <c r="AN30" s="17"/>
-      <c r="AO30" s="30">
+      <c r="AO30" s="29">
         <v>10</v>
       </c>
-      <c r="AP30" s="17"/>
-      <c r="AQ30" s="17"/>
-      <c r="AR30" s="17"/>
-      <c r="AS30" s="17"/>
-      <c r="AT30" s="17"/>
-      <c r="AU30" s="17"/>
-      <c r="AV30" s="17"/>
-      <c r="AW30" s="17"/>
-      <c r="AX30" s="17"/>
-      <c r="AY30" s="17"/>
-      <c r="AZ30" s="17"/>
-      <c r="BA30" s="17"/>
-      <c r="BB30" s="17"/>
-      <c r="BC30" s="17"/>
-      <c r="BD30" s="17"/>
-      <c r="BE30" s="17"/>
-      <c r="BF30" s="17"/>
-      <c r="BG30" s="17"/>
-      <c r="BH30" s="17"/>
-      <c r="BI30" s="17"/>
-      <c r="BJ30" s="17"/>
-      <c r="BK30" s="17"/>
-      <c r="BL30" s="17"/>
-      <c r="BM30" s="17"/>
-      <c r="BN30" s="17"/>
-      <c r="BO30" s="17"/>
-      <c r="BP30" s="17"/>
-      <c r="BQ30" s="17"/>
-      <c r="BR30" s="17"/>
-      <c r="BS30" s="17"/>
-      <c r="BT30" s="17"/>
-      <c r="BU30" s="17"/>
-      <c r="BV30" s="17"/>
-      <c r="BW30" s="17"/>
-      <c r="BX30" s="17"/>
-      <c r="BY30" s="17"/>
-      <c r="BZ30" s="17"/>
-      <c r="CA30" s="17"/>
+      <c r="AP30" s="30"/>
+      <c r="AQ30" s="30"/>
+      <c r="AR30" s="30"/>
+      <c r="AS30" s="30"/>
+      <c r="AT30" s="30"/>
+      <c r="AU30" s="30"/>
+      <c r="AV30" s="30"/>
+      <c r="AW30" s="30"/>
+      <c r="AX30" s="30"/>
+      <c r="AY30" s="30"/>
+      <c r="AZ30" s="30"/>
+      <c r="BA30" s="30"/>
+      <c r="BB30" s="30"/>
+      <c r="BC30" s="30"/>
+      <c r="BD30" s="30"/>
+      <c r="BE30" s="30"/>
+      <c r="BF30" s="30"/>
+      <c r="BG30" s="30"/>
+      <c r="BH30" s="30"/>
+      <c r="BI30" s="30"/>
+      <c r="BJ30" s="30"/>
+      <c r="BK30" s="30"/>
+      <c r="BL30" s="30"/>
+      <c r="BM30" s="30"/>
+      <c r="BN30" s="30"/>
+      <c r="BO30" s="30"/>
+      <c r="BP30" s="30"/>
+      <c r="BQ30" s="30"/>
+      <c r="BR30" s="30"/>
+      <c r="BS30" s="30"/>
+      <c r="BT30" s="30"/>
+      <c r="BU30" s="30"/>
+      <c r="BV30" s="30"/>
+      <c r="BW30" s="30"/>
+      <c r="BX30" s="30"/>
+      <c r="BY30" s="30"/>
+      <c r="BZ30" s="30"/>
+      <c r="CA30" s="30"/>
       <c r="CB30" s="5"/>
       <c r="CC30" s="22"/>
       <c r="CD30" s="33"/>
@@ -8469,46 +8498,46 @@
       <c r="DO30" s="17"/>
       <c r="DP30" s="17"/>
       <c r="DQ30" s="17"/>
-      <c r="DR30" s="30">
+      <c r="DR30" s="29">
         <v>10</v>
       </c>
-      <c r="DS30" s="17"/>
-      <c r="DT30" s="17"/>
-      <c r="DU30" s="17"/>
-      <c r="DV30" s="17"/>
-      <c r="DW30" s="17"/>
-      <c r="DX30" s="17"/>
-      <c r="DY30" s="17"/>
-      <c r="DZ30" s="17"/>
-      <c r="EA30" s="17"/>
-      <c r="EB30" s="17"/>
-      <c r="EC30" s="17"/>
-      <c r="ED30" s="17"/>
-      <c r="EE30" s="17"/>
-      <c r="EF30" s="17"/>
-      <c r="EG30" s="17"/>
-      <c r="EH30" s="17"/>
-      <c r="EI30" s="17"/>
-      <c r="EJ30" s="17"/>
-      <c r="EK30" s="17"/>
-      <c r="EL30" s="17"/>
-      <c r="EM30" s="17"/>
-      <c r="EN30" s="17"/>
-      <c r="EO30" s="17"/>
-      <c r="EP30" s="17"/>
-      <c r="EQ30" s="17"/>
-      <c r="ER30" s="17"/>
-      <c r="ES30" s="17"/>
-      <c r="ET30" s="17"/>
-      <c r="EU30" s="17"/>
-      <c r="EV30" s="17"/>
-      <c r="EW30" s="17"/>
-      <c r="EX30" s="17"/>
-      <c r="EY30" s="17"/>
-      <c r="EZ30" s="17"/>
-      <c r="FA30" s="17"/>
-      <c r="FB30" s="17"/>
-      <c r="FC30" s="17"/>
+      <c r="DS30" s="30"/>
+      <c r="DT30" s="30"/>
+      <c r="DU30" s="30"/>
+      <c r="DV30" s="30"/>
+      <c r="DW30" s="30"/>
+      <c r="DX30" s="30"/>
+      <c r="DY30" s="30"/>
+      <c r="DZ30" s="30"/>
+      <c r="EA30" s="30"/>
+      <c r="EB30" s="30"/>
+      <c r="EC30" s="30"/>
+      <c r="ED30" s="30"/>
+      <c r="EE30" s="30"/>
+      <c r="EF30" s="30"/>
+      <c r="EG30" s="30"/>
+      <c r="EH30" s="30"/>
+      <c r="EI30" s="30"/>
+      <c r="EJ30" s="30"/>
+      <c r="EK30" s="30"/>
+      <c r="EL30" s="30"/>
+      <c r="EM30" s="30"/>
+      <c r="EN30" s="30"/>
+      <c r="EO30" s="30"/>
+      <c r="EP30" s="30"/>
+      <c r="EQ30" s="30"/>
+      <c r="ER30" s="30"/>
+      <c r="ES30" s="30"/>
+      <c r="ET30" s="30"/>
+      <c r="EU30" s="30"/>
+      <c r="EV30" s="30"/>
+      <c r="EW30" s="30"/>
+      <c r="EX30" s="30"/>
+      <c r="EY30" s="30"/>
+      <c r="EZ30" s="30"/>
+      <c r="FA30" s="30"/>
+      <c r="FB30" s="30"/>
+      <c r="FC30" s="30"/>
       <c r="FD30" s="24"/>
     </row>
     <row r="31" customHeight="1" spans="2:160">
@@ -8555,47 +8584,47 @@
       <c r="AL31" s="17"/>
       <c r="AM31" s="17"/>
       <c r="AN31" s="17"/>
-      <c r="AO31" s="30">
+      <c r="AO31" s="29">
         <v>11</v>
       </c>
-      <c r="AP31" s="17"/>
-      <c r="AQ31" s="17"/>
-      <c r="AR31" s="17"/>
-      <c r="AS31" s="17"/>
-      <c r="AT31" s="17"/>
-      <c r="AU31" s="17"/>
-      <c r="AV31" s="17"/>
-      <c r="AW31" s="17"/>
-      <c r="AX31" s="17"/>
-      <c r="AY31" s="17"/>
-      <c r="AZ31" s="17"/>
-      <c r="BA31" s="17"/>
-      <c r="BB31" s="17"/>
-      <c r="BC31" s="17"/>
-      <c r="BD31" s="17"/>
-      <c r="BE31" s="17"/>
-      <c r="BF31" s="17"/>
-      <c r="BG31" s="17"/>
-      <c r="BH31" s="17"/>
-      <c r="BI31" s="17"/>
-      <c r="BJ31" s="17"/>
-      <c r="BK31" s="17"/>
-      <c r="BL31" s="17"/>
-      <c r="BM31" s="17"/>
-      <c r="BN31" s="17"/>
-      <c r="BO31" s="17"/>
-      <c r="BP31" s="17"/>
-      <c r="BQ31" s="17"/>
-      <c r="BR31" s="17"/>
-      <c r="BS31" s="17"/>
-      <c r="BT31" s="17"/>
-      <c r="BU31" s="17"/>
-      <c r="BV31" s="17"/>
-      <c r="BW31" s="17"/>
-      <c r="BX31" s="17"/>
-      <c r="BY31" s="17"/>
-      <c r="BZ31" s="17"/>
-      <c r="CA31" s="17"/>
+      <c r="AP31" s="30"/>
+      <c r="AQ31" s="30"/>
+      <c r="AR31" s="30"/>
+      <c r="AS31" s="30"/>
+      <c r="AT31" s="30"/>
+      <c r="AU31" s="30"/>
+      <c r="AV31" s="30"/>
+      <c r="AW31" s="30"/>
+      <c r="AX31" s="30"/>
+      <c r="AY31" s="30"/>
+      <c r="AZ31" s="30"/>
+      <c r="BA31" s="30"/>
+      <c r="BB31" s="30"/>
+      <c r="BC31" s="30"/>
+      <c r="BD31" s="30"/>
+      <c r="BE31" s="30"/>
+      <c r="BF31" s="30"/>
+      <c r="BG31" s="30"/>
+      <c r="BH31" s="30"/>
+      <c r="BI31" s="30"/>
+      <c r="BJ31" s="30"/>
+      <c r="BK31" s="30"/>
+      <c r="BL31" s="30"/>
+      <c r="BM31" s="30"/>
+      <c r="BN31" s="30"/>
+      <c r="BO31" s="30"/>
+      <c r="BP31" s="30"/>
+      <c r="BQ31" s="30"/>
+      <c r="BR31" s="30"/>
+      <c r="BS31" s="30"/>
+      <c r="BT31" s="30"/>
+      <c r="BU31" s="30"/>
+      <c r="BV31" s="30"/>
+      <c r="BW31" s="30"/>
+      <c r="BX31" s="30"/>
+      <c r="BY31" s="30"/>
+      <c r="BZ31" s="30"/>
+      <c r="CA31" s="30"/>
       <c r="CB31" s="5"/>
       <c r="CC31" s="22"/>
       <c r="CD31" s="33"/>
@@ -8640,46 +8669,46 @@
       <c r="DO31" s="17"/>
       <c r="DP31" s="17"/>
       <c r="DQ31" s="17"/>
-      <c r="DR31" s="30">
+      <c r="DR31" s="29">
         <v>11</v>
       </c>
-      <c r="DS31" s="17"/>
-      <c r="DT31" s="17"/>
-      <c r="DU31" s="17"/>
-      <c r="DV31" s="17"/>
-      <c r="DW31" s="17"/>
-      <c r="DX31" s="17"/>
-      <c r="DY31" s="17"/>
-      <c r="DZ31" s="17"/>
-      <c r="EA31" s="17"/>
-      <c r="EB31" s="17"/>
-      <c r="EC31" s="17"/>
-      <c r="ED31" s="17"/>
-      <c r="EE31" s="17"/>
-      <c r="EF31" s="17"/>
-      <c r="EG31" s="17"/>
-      <c r="EH31" s="17"/>
-      <c r="EI31" s="17"/>
-      <c r="EJ31" s="17"/>
-      <c r="EK31" s="17"/>
-      <c r="EL31" s="17"/>
-      <c r="EM31" s="17"/>
-      <c r="EN31" s="17"/>
-      <c r="EO31" s="17"/>
-      <c r="EP31" s="17"/>
-      <c r="EQ31" s="17"/>
-      <c r="ER31" s="17"/>
-      <c r="ES31" s="17"/>
-      <c r="ET31" s="17"/>
-      <c r="EU31" s="17"/>
-      <c r="EV31" s="17"/>
-      <c r="EW31" s="17"/>
-      <c r="EX31" s="17"/>
-      <c r="EY31" s="17"/>
-      <c r="EZ31" s="17"/>
-      <c r="FA31" s="17"/>
-      <c r="FB31" s="17"/>
-      <c r="FC31" s="17"/>
+      <c r="DS31" s="30"/>
+      <c r="DT31" s="30"/>
+      <c r="DU31" s="30"/>
+      <c r="DV31" s="30"/>
+      <c r="DW31" s="30"/>
+      <c r="DX31" s="30"/>
+      <c r="DY31" s="30"/>
+      <c r="DZ31" s="30"/>
+      <c r="EA31" s="30"/>
+      <c r="EB31" s="30"/>
+      <c r="EC31" s="30"/>
+      <c r="ED31" s="30"/>
+      <c r="EE31" s="30"/>
+      <c r="EF31" s="30"/>
+      <c r="EG31" s="30"/>
+      <c r="EH31" s="30"/>
+      <c r="EI31" s="30"/>
+      <c r="EJ31" s="30"/>
+      <c r="EK31" s="30"/>
+      <c r="EL31" s="30"/>
+      <c r="EM31" s="30"/>
+      <c r="EN31" s="30"/>
+      <c r="EO31" s="30"/>
+      <c r="EP31" s="30"/>
+      <c r="EQ31" s="30"/>
+      <c r="ER31" s="30"/>
+      <c r="ES31" s="30"/>
+      <c r="ET31" s="30"/>
+      <c r="EU31" s="30"/>
+      <c r="EV31" s="30"/>
+      <c r="EW31" s="30"/>
+      <c r="EX31" s="30"/>
+      <c r="EY31" s="30"/>
+      <c r="EZ31" s="30"/>
+      <c r="FA31" s="30"/>
+      <c r="FB31" s="30"/>
+      <c r="FC31" s="30"/>
       <c r="FD31" s="24"/>
     </row>
     <row r="32" customHeight="1" spans="2:160">
@@ -8724,47 +8753,47 @@
       <c r="AL32" s="17"/>
       <c r="AM32" s="17"/>
       <c r="AN32" s="17"/>
-      <c r="AO32" s="30">
+      <c r="AO32" s="29">
         <v>12</v>
       </c>
-      <c r="AP32" s="17"/>
-      <c r="AQ32" s="17"/>
-      <c r="AR32" s="17"/>
-      <c r="AS32" s="17"/>
-      <c r="AT32" s="17"/>
-      <c r="AU32" s="17"/>
-      <c r="AV32" s="17"/>
-      <c r="AW32" s="17"/>
-      <c r="AX32" s="17"/>
-      <c r="AY32" s="17"/>
-      <c r="AZ32" s="17"/>
-      <c r="BA32" s="17"/>
-      <c r="BB32" s="17"/>
-      <c r="BC32" s="17"/>
-      <c r="BD32" s="17"/>
-      <c r="BE32" s="17"/>
-      <c r="BF32" s="17"/>
-      <c r="BG32" s="17"/>
-      <c r="BH32" s="17"/>
-      <c r="BI32" s="17"/>
-      <c r="BJ32" s="17"/>
-      <c r="BK32" s="17"/>
-      <c r="BL32" s="17"/>
-      <c r="BM32" s="17"/>
-      <c r="BN32" s="17"/>
-      <c r="BO32" s="17"/>
-      <c r="BP32" s="17"/>
-      <c r="BQ32" s="17"/>
-      <c r="BR32" s="17"/>
-      <c r="BS32" s="17"/>
-      <c r="BT32" s="17"/>
-      <c r="BU32" s="17"/>
-      <c r="BV32" s="17"/>
-      <c r="BW32" s="17"/>
-      <c r="BX32" s="17"/>
-      <c r="BY32" s="17"/>
-      <c r="BZ32" s="17"/>
-      <c r="CA32" s="17"/>
+      <c r="AP32" s="30"/>
+      <c r="AQ32" s="30"/>
+      <c r="AR32" s="30"/>
+      <c r="AS32" s="30"/>
+      <c r="AT32" s="30"/>
+      <c r="AU32" s="30"/>
+      <c r="AV32" s="30"/>
+      <c r="AW32" s="30"/>
+      <c r="AX32" s="30"/>
+      <c r="AY32" s="30"/>
+      <c r="AZ32" s="30"/>
+      <c r="BA32" s="30"/>
+      <c r="BB32" s="30"/>
+      <c r="BC32" s="30"/>
+      <c r="BD32" s="30"/>
+      <c r="BE32" s="30"/>
+      <c r="BF32" s="30"/>
+      <c r="BG32" s="30"/>
+      <c r="BH32" s="30"/>
+      <c r="BI32" s="30"/>
+      <c r="BJ32" s="30"/>
+      <c r="BK32" s="30"/>
+      <c r="BL32" s="30"/>
+      <c r="BM32" s="30"/>
+      <c r="BN32" s="30"/>
+      <c r="BO32" s="30"/>
+      <c r="BP32" s="30"/>
+      <c r="BQ32" s="30"/>
+      <c r="BR32" s="30"/>
+      <c r="BS32" s="30"/>
+      <c r="BT32" s="30"/>
+      <c r="BU32" s="30"/>
+      <c r="BV32" s="30"/>
+      <c r="BW32" s="30"/>
+      <c r="BX32" s="30"/>
+      <c r="BY32" s="30"/>
+      <c r="BZ32" s="30"/>
+      <c r="CA32" s="30"/>
       <c r="CB32" s="5"/>
       <c r="CC32" s="22"/>
       <c r="CD32" s="33"/>
@@ -8809,46 +8838,46 @@
       <c r="DO32" s="17"/>
       <c r="DP32" s="17"/>
       <c r="DQ32" s="17"/>
-      <c r="DR32" s="30">
+      <c r="DR32" s="29">
         <v>12</v>
       </c>
-      <c r="DS32" s="17"/>
-      <c r="DT32" s="17"/>
-      <c r="DU32" s="17"/>
-      <c r="DV32" s="17"/>
-      <c r="DW32" s="17"/>
-      <c r="DX32" s="17"/>
-      <c r="DY32" s="17"/>
-      <c r="DZ32" s="17"/>
-      <c r="EA32" s="17"/>
-      <c r="EB32" s="17"/>
-      <c r="EC32" s="17"/>
-      <c r="ED32" s="17"/>
-      <c r="EE32" s="17"/>
-      <c r="EF32" s="17"/>
-      <c r="EG32" s="17"/>
-      <c r="EH32" s="17"/>
-      <c r="EI32" s="17"/>
-      <c r="EJ32" s="17"/>
-      <c r="EK32" s="17"/>
-      <c r="EL32" s="17"/>
-      <c r="EM32" s="17"/>
-      <c r="EN32" s="17"/>
-      <c r="EO32" s="17"/>
-      <c r="EP32" s="17"/>
-      <c r="EQ32" s="17"/>
-      <c r="ER32" s="17"/>
-      <c r="ES32" s="17"/>
-      <c r="ET32" s="17"/>
-      <c r="EU32" s="17"/>
-      <c r="EV32" s="17"/>
-      <c r="EW32" s="17"/>
-      <c r="EX32" s="17"/>
-      <c r="EY32" s="17"/>
-      <c r="EZ32" s="17"/>
-      <c r="FA32" s="17"/>
-      <c r="FB32" s="17"/>
-      <c r="FC32" s="17"/>
+      <c r="DS32" s="30"/>
+      <c r="DT32" s="30"/>
+      <c r="DU32" s="30"/>
+      <c r="DV32" s="30"/>
+      <c r="DW32" s="30"/>
+      <c r="DX32" s="30"/>
+      <c r="DY32" s="30"/>
+      <c r="DZ32" s="30"/>
+      <c r="EA32" s="30"/>
+      <c r="EB32" s="30"/>
+      <c r="EC32" s="30"/>
+      <c r="ED32" s="30"/>
+      <c r="EE32" s="30"/>
+      <c r="EF32" s="30"/>
+      <c r="EG32" s="30"/>
+      <c r="EH32" s="30"/>
+      <c r="EI32" s="30"/>
+      <c r="EJ32" s="30"/>
+      <c r="EK32" s="30"/>
+      <c r="EL32" s="30"/>
+      <c r="EM32" s="30"/>
+      <c r="EN32" s="30"/>
+      <c r="EO32" s="30"/>
+      <c r="EP32" s="30"/>
+      <c r="EQ32" s="30"/>
+      <c r="ER32" s="30"/>
+      <c r="ES32" s="30"/>
+      <c r="ET32" s="30"/>
+      <c r="EU32" s="30"/>
+      <c r="EV32" s="30"/>
+      <c r="EW32" s="30"/>
+      <c r="EX32" s="30"/>
+      <c r="EY32" s="30"/>
+      <c r="EZ32" s="30"/>
+      <c r="FA32" s="30"/>
+      <c r="FB32" s="30"/>
+      <c r="FC32" s="30"/>
       <c r="FD32" s="24"/>
     </row>
     <row r="33" customHeight="1" spans="2:160">
@@ -8893,47 +8922,47 @@
       <c r="AL33" s="17"/>
       <c r="AM33" s="17"/>
       <c r="AN33" s="17"/>
-      <c r="AO33" s="30">
+      <c r="AO33" s="29">
         <v>13</v>
       </c>
-      <c r="AP33" s="17"/>
-      <c r="AQ33" s="17"/>
-      <c r="AR33" s="17"/>
-      <c r="AS33" s="17"/>
-      <c r="AT33" s="17"/>
-      <c r="AU33" s="17"/>
-      <c r="AV33" s="17"/>
-      <c r="AW33" s="17"/>
-      <c r="AX33" s="17"/>
-      <c r="AY33" s="17"/>
-      <c r="AZ33" s="17"/>
-      <c r="BA33" s="17"/>
-      <c r="BB33" s="17"/>
-      <c r="BC33" s="17"/>
-      <c r="BD33" s="17"/>
-      <c r="BE33" s="17"/>
-      <c r="BF33" s="17"/>
-      <c r="BG33" s="17"/>
-      <c r="BH33" s="17"/>
-      <c r="BI33" s="17"/>
-      <c r="BJ33" s="17"/>
-      <c r="BK33" s="17"/>
-      <c r="BL33" s="17"/>
-      <c r="BM33" s="17"/>
-      <c r="BN33" s="17"/>
-      <c r="BO33" s="17"/>
-      <c r="BP33" s="17"/>
-      <c r="BQ33" s="17"/>
-      <c r="BR33" s="17"/>
-      <c r="BS33" s="17"/>
-      <c r="BT33" s="17"/>
-      <c r="BU33" s="17"/>
-      <c r="BV33" s="17"/>
-      <c r="BW33" s="17"/>
-      <c r="BX33" s="17"/>
-      <c r="BY33" s="17"/>
-      <c r="BZ33" s="17"/>
-      <c r="CA33" s="17"/>
+      <c r="AP33" s="30"/>
+      <c r="AQ33" s="30"/>
+      <c r="AR33" s="30"/>
+      <c r="AS33" s="30"/>
+      <c r="AT33" s="30"/>
+      <c r="AU33" s="30"/>
+      <c r="AV33" s="30"/>
+      <c r="AW33" s="30"/>
+      <c r="AX33" s="30"/>
+      <c r="AY33" s="30"/>
+      <c r="AZ33" s="30"/>
+      <c r="BA33" s="30"/>
+      <c r="BB33" s="30"/>
+      <c r="BC33" s="30"/>
+      <c r="BD33" s="30"/>
+      <c r="BE33" s="30"/>
+      <c r="BF33" s="30"/>
+      <c r="BG33" s="30"/>
+      <c r="BH33" s="30"/>
+      <c r="BI33" s="30"/>
+      <c r="BJ33" s="30"/>
+      <c r="BK33" s="30"/>
+      <c r="BL33" s="30"/>
+      <c r="BM33" s="30"/>
+      <c r="BN33" s="30"/>
+      <c r="BO33" s="30"/>
+      <c r="BP33" s="30"/>
+      <c r="BQ33" s="30"/>
+      <c r="BR33" s="30"/>
+      <c r="BS33" s="30"/>
+      <c r="BT33" s="30"/>
+      <c r="BU33" s="30"/>
+      <c r="BV33" s="30"/>
+      <c r="BW33" s="30"/>
+      <c r="BX33" s="30"/>
+      <c r="BY33" s="30"/>
+      <c r="BZ33" s="30"/>
+      <c r="CA33" s="30"/>
       <c r="CB33" s="5"/>
       <c r="CC33" s="22"/>
       <c r="CD33" s="33"/>
@@ -8978,46 +9007,46 @@
       <c r="DO33" s="17"/>
       <c r="DP33" s="17"/>
       <c r="DQ33" s="17"/>
-      <c r="DR33" s="30">
+      <c r="DR33" s="29">
         <v>13</v>
       </c>
-      <c r="DS33" s="17"/>
-      <c r="DT33" s="17"/>
-      <c r="DU33" s="17"/>
-      <c r="DV33" s="17"/>
-      <c r="DW33" s="17"/>
-      <c r="DX33" s="17"/>
-      <c r="DY33" s="17"/>
-      <c r="DZ33" s="17"/>
-      <c r="EA33" s="17"/>
-      <c r="EB33" s="17"/>
-      <c r="EC33" s="17"/>
-      <c r="ED33" s="17"/>
-      <c r="EE33" s="17"/>
-      <c r="EF33" s="17"/>
-      <c r="EG33" s="17"/>
-      <c r="EH33" s="17"/>
-      <c r="EI33" s="17"/>
-      <c r="EJ33" s="17"/>
-      <c r="EK33" s="17"/>
-      <c r="EL33" s="17"/>
-      <c r="EM33" s="17"/>
-      <c r="EN33" s="17"/>
-      <c r="EO33" s="17"/>
-      <c r="EP33" s="17"/>
-      <c r="EQ33" s="17"/>
-      <c r="ER33" s="17"/>
-      <c r="ES33" s="17"/>
-      <c r="ET33" s="17"/>
-      <c r="EU33" s="17"/>
-      <c r="EV33" s="17"/>
-      <c r="EW33" s="17"/>
-      <c r="EX33" s="17"/>
-      <c r="EY33" s="17"/>
-      <c r="EZ33" s="17"/>
-      <c r="FA33" s="17"/>
-      <c r="FB33" s="17"/>
-      <c r="FC33" s="17"/>
+      <c r="DS33" s="30"/>
+      <c r="DT33" s="30"/>
+      <c r="DU33" s="30"/>
+      <c r="DV33" s="30"/>
+      <c r="DW33" s="30"/>
+      <c r="DX33" s="30"/>
+      <c r="DY33" s="30"/>
+      <c r="DZ33" s="30"/>
+      <c r="EA33" s="30"/>
+      <c r="EB33" s="30"/>
+      <c r="EC33" s="30"/>
+      <c r="ED33" s="30"/>
+      <c r="EE33" s="30"/>
+      <c r="EF33" s="30"/>
+      <c r="EG33" s="30"/>
+      <c r="EH33" s="30"/>
+      <c r="EI33" s="30"/>
+      <c r="EJ33" s="30"/>
+      <c r="EK33" s="30"/>
+      <c r="EL33" s="30"/>
+      <c r="EM33" s="30"/>
+      <c r="EN33" s="30"/>
+      <c r="EO33" s="30"/>
+      <c r="EP33" s="30"/>
+      <c r="EQ33" s="30"/>
+      <c r="ER33" s="30"/>
+      <c r="ES33" s="30"/>
+      <c r="ET33" s="30"/>
+      <c r="EU33" s="30"/>
+      <c r="EV33" s="30"/>
+      <c r="EW33" s="30"/>
+      <c r="EX33" s="30"/>
+      <c r="EY33" s="30"/>
+      <c r="EZ33" s="30"/>
+      <c r="FA33" s="30"/>
+      <c r="FB33" s="30"/>
+      <c r="FC33" s="30"/>
       <c r="FD33" s="24"/>
     </row>
     <row r="34" customHeight="1" spans="2:160">
@@ -9062,47 +9091,47 @@
       <c r="AL34" s="17"/>
       <c r="AM34" s="17"/>
       <c r="AN34" s="17"/>
-      <c r="AO34" s="30">
+      <c r="AO34" s="29">
         <v>14</v>
       </c>
-      <c r="AP34" s="17"/>
-      <c r="AQ34" s="17"/>
-      <c r="AR34" s="17"/>
-      <c r="AS34" s="17"/>
-      <c r="AT34" s="17"/>
-      <c r="AU34" s="17"/>
-      <c r="AV34" s="17"/>
-      <c r="AW34" s="17"/>
-      <c r="AX34" s="17"/>
-      <c r="AY34" s="17"/>
-      <c r="AZ34" s="17"/>
-      <c r="BA34" s="17"/>
-      <c r="BB34" s="17"/>
-      <c r="BC34" s="17"/>
-      <c r="BD34" s="17"/>
-      <c r="BE34" s="17"/>
-      <c r="BF34" s="17"/>
-      <c r="BG34" s="17"/>
-      <c r="BH34" s="17"/>
-      <c r="BI34" s="17"/>
-      <c r="BJ34" s="17"/>
-      <c r="BK34" s="17"/>
-      <c r="BL34" s="17"/>
-      <c r="BM34" s="17"/>
-      <c r="BN34" s="17"/>
-      <c r="BO34" s="17"/>
-      <c r="BP34" s="17"/>
-      <c r="BQ34" s="17"/>
-      <c r="BR34" s="17"/>
-      <c r="BS34" s="17"/>
-      <c r="BT34" s="17"/>
-      <c r="BU34" s="17"/>
-      <c r="BV34" s="17"/>
-      <c r="BW34" s="17"/>
-      <c r="BX34" s="17"/>
-      <c r="BY34" s="17"/>
-      <c r="BZ34" s="17"/>
-      <c r="CA34" s="17"/>
+      <c r="AP34" s="30"/>
+      <c r="AQ34" s="30"/>
+      <c r="AR34" s="30"/>
+      <c r="AS34" s="30"/>
+      <c r="AT34" s="30"/>
+      <c r="AU34" s="30"/>
+      <c r="AV34" s="30"/>
+      <c r="AW34" s="30"/>
+      <c r="AX34" s="30"/>
+      <c r="AY34" s="30"/>
+      <c r="AZ34" s="30"/>
+      <c r="BA34" s="30"/>
+      <c r="BB34" s="30"/>
+      <c r="BC34" s="30"/>
+      <c r="BD34" s="30"/>
+      <c r="BE34" s="30"/>
+      <c r="BF34" s="30"/>
+      <c r="BG34" s="30"/>
+      <c r="BH34" s="30"/>
+      <c r="BI34" s="30"/>
+      <c r="BJ34" s="30"/>
+      <c r="BK34" s="30"/>
+      <c r="BL34" s="30"/>
+      <c r="BM34" s="30"/>
+      <c r="BN34" s="30"/>
+      <c r="BO34" s="30"/>
+      <c r="BP34" s="30"/>
+      <c r="BQ34" s="30"/>
+      <c r="BR34" s="30"/>
+      <c r="BS34" s="30"/>
+      <c r="BT34" s="30"/>
+      <c r="BU34" s="30"/>
+      <c r="BV34" s="30"/>
+      <c r="BW34" s="30"/>
+      <c r="BX34" s="30"/>
+      <c r="BY34" s="30"/>
+      <c r="BZ34" s="30"/>
+      <c r="CA34" s="30"/>
       <c r="CB34" s="5"/>
       <c r="CC34" s="22"/>
       <c r="CD34" s="33"/>
@@ -9147,46 +9176,46 @@
       <c r="DO34" s="17"/>
       <c r="DP34" s="17"/>
       <c r="DQ34" s="17"/>
-      <c r="DR34" s="30">
+      <c r="DR34" s="29">
         <v>14</v>
       </c>
-      <c r="DS34" s="17"/>
-      <c r="DT34" s="17"/>
-      <c r="DU34" s="17"/>
-      <c r="DV34" s="17"/>
-      <c r="DW34" s="17"/>
-      <c r="DX34" s="17"/>
-      <c r="DY34" s="17"/>
-      <c r="DZ34" s="17"/>
-      <c r="EA34" s="17"/>
-      <c r="EB34" s="17"/>
-      <c r="EC34" s="17"/>
-      <c r="ED34" s="17"/>
-      <c r="EE34" s="17"/>
-      <c r="EF34" s="17"/>
-      <c r="EG34" s="17"/>
-      <c r="EH34" s="17"/>
-      <c r="EI34" s="17"/>
-      <c r="EJ34" s="17"/>
-      <c r="EK34" s="17"/>
-      <c r="EL34" s="17"/>
-      <c r="EM34" s="17"/>
-      <c r="EN34" s="17"/>
-      <c r="EO34" s="17"/>
-      <c r="EP34" s="17"/>
-      <c r="EQ34" s="17"/>
-      <c r="ER34" s="17"/>
-      <c r="ES34" s="17"/>
-      <c r="ET34" s="17"/>
-      <c r="EU34" s="17"/>
-      <c r="EV34" s="17"/>
-      <c r="EW34" s="17"/>
-      <c r="EX34" s="17"/>
-      <c r="EY34" s="17"/>
-      <c r="EZ34" s="17"/>
-      <c r="FA34" s="17"/>
-      <c r="FB34" s="17"/>
-      <c r="FC34" s="17"/>
+      <c r="DS34" s="30"/>
+      <c r="DT34" s="30"/>
+      <c r="DU34" s="30"/>
+      <c r="DV34" s="30"/>
+      <c r="DW34" s="30"/>
+      <c r="DX34" s="30"/>
+      <c r="DY34" s="30"/>
+      <c r="DZ34" s="30"/>
+      <c r="EA34" s="30"/>
+      <c r="EB34" s="30"/>
+      <c r="EC34" s="30"/>
+      <c r="ED34" s="30"/>
+      <c r="EE34" s="30"/>
+      <c r="EF34" s="30"/>
+      <c r="EG34" s="30"/>
+      <c r="EH34" s="30"/>
+      <c r="EI34" s="30"/>
+      <c r="EJ34" s="30"/>
+      <c r="EK34" s="30"/>
+      <c r="EL34" s="30"/>
+      <c r="EM34" s="30"/>
+      <c r="EN34" s="30"/>
+      <c r="EO34" s="30"/>
+      <c r="EP34" s="30"/>
+      <c r="EQ34" s="30"/>
+      <c r="ER34" s="30"/>
+      <c r="ES34" s="30"/>
+      <c r="ET34" s="30"/>
+      <c r="EU34" s="30"/>
+      <c r="EV34" s="30"/>
+      <c r="EW34" s="30"/>
+      <c r="EX34" s="30"/>
+      <c r="EY34" s="30"/>
+      <c r="EZ34" s="30"/>
+      <c r="FA34" s="30"/>
+      <c r="FB34" s="30"/>
+      <c r="FC34" s="30"/>
       <c r="FD34" s="24"/>
     </row>
     <row r="35" customHeight="1" spans="2:160">
@@ -9419,7 +9448,7 @@
       <c r="CR37" s="33"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" selectLockedCells="1" objects="1" scenarios="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <mergeCells count="106">
     <mergeCell ref="V3:BI3"/>
     <mergeCell ref="BR3:CR3"/>

</xml_diff>